<commit_message>
replaced xlstotsv with cleandata using more brenninc utils
</commit_message>
<xml_diff>
--- a/repr_tools/test-data/mini.xlsx
+++ b/repr_tools/test-data/mini.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>A</t>
   </si>
@@ -210,7 +210,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -284,9 +284,6 @@
       <c r="C10" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="E10" s="0" t="s">
         <v>15</v>
       </c>
@@ -305,7 +302,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>19</v>
@@ -323,9 +320,6 @@
       </c>
       <c r="C12" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>9</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>20</v>

</xml_diff>